<commit_message>
fastapi and streamlit working
</commit_message>
<xml_diff>
--- a/data/test_applications/approved_1/assets_liabilities.xlsx
+++ b/data/test_applications/approved_1/assets_liabilities.xlsx
@@ -89,7 +89,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,12 +106,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -234,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -257,7 +251,7 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -269,9 +263,6 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -281,19 +272,13 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -608,24 +593,24 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="10" width="25.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="21" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="18" width="20.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="B1" s="16"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="6"/>
-      <c r="B2" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+      <c r="B2" s="16"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>16</v>
       </c>
     </row>
@@ -633,19 +618,19 @@
       <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="8">
         <v>4200</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="6"/>
-      <c r="B5" s="17"/>
+      <c r="B5" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="8">
         <v>5104</v>
       </c>
     </row>
@@ -653,7 +638,7 @@
       <c r="A7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="8">
         <v>110725</v>
       </c>
     </row>
@@ -661,7 +646,7 @@
       <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="17">
         <v>-105621</v>
       </c>
     </row>
@@ -669,7 +654,7 @@
       <c r="A9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="16">
         <v>0.05</v>
       </c>
     </row>
@@ -698,13 +683,13 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>10</v>
       </c>
     </row>
@@ -724,7 +709,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="6"/>
-      <c r="C3" s="15">
+      <c r="C3" s="14">
         <v>5104</v>
       </c>
     </row>
@@ -747,8 +732,8 @@
     <col min="1" max="1" style="9" width="20.005" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="10" width="25.005" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="11" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="11" width="18.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="11" width="16.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">

</xml_diff>